<commit_message>
email request for prac data
</commit_message>
<xml_diff>
--- a/01 background/Analysis_Specifications_20220913.xlsx
+++ b/01 background/Analysis_Specifications_20220913.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\FHPC\DATA\HCPF_Data_files_SECURE\Kim\isp\isp_utilization\01 background\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0D2BE5-235C-4AFB-B789-015210F01674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D0DD31-F4AD-4E36-9E07-40F16341CA8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{A163DE94-6307-4150-BFFB-6B4CE85967AB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5124" xr2:uid="{A163DE94-6307-4150-BFFB-6B4CE85967AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Specs" sheetId="2" r:id="rId1"/>
@@ -28,8 +28,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C548FC-D9C9-4889-90CA-494B21B536C4}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89965000-8AB6-4737-B675-CEC9CFAF2AB6}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>